<commit_message>
final code for paper submission
</commit_message>
<xml_diff>
--- a/in_vitro_heatmaps_scatter_plots/input/Supplementary_Table_6.xlsx
+++ b/in_vitro_heatmaps_scatter_plots/input/Supplementary_Table_6.xlsx
@@ -4,17 +4,18 @@
   <fileVersion appName="xl" lastEdited="5" lowestEdited="5" rupBuild="28705"/>
   <workbookPr showInkAnnotation="0" autoCompressPictures="0"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="38400" windowHeight="20820" tabRatio="500" activeTab="4"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="38400" windowHeight="20820" tabRatio="500"/>
   </bookViews>
   <sheets>
-    <sheet name="cultures" sheetId="18" r:id="rId1"/>
-    <sheet name="full_taxonomy" sheetId="19" r:id="rId2"/>
-    <sheet name="v4_16s" sheetId="20" r:id="rId3"/>
-    <sheet name="full_length_16s" sheetId="21" r:id="rId4"/>
-    <sheet name="media" sheetId="22" r:id="rId5"/>
+    <sheet name="strains_with_data" sheetId="23" r:id="rId1"/>
+    <sheet name="cultures" sheetId="18" r:id="rId2"/>
+    <sheet name="full_taxonomy" sheetId="19" r:id="rId3"/>
+    <sheet name="v4_16s" sheetId="20" r:id="rId4"/>
+    <sheet name="full_length_16s" sheetId="21" r:id="rId5"/>
+    <sheet name="media" sheetId="22" r:id="rId6"/>
   </sheets>
   <definedNames>
-    <definedName name="_xlnm._FilterDatabase" localSheetId="1" hidden="1">full_taxonomy!$A$1:$O$256</definedName>
+    <definedName name="_xlnm._FilterDatabase" localSheetId="2" hidden="1">full_taxonomy!$A$1:$O$256</definedName>
   </definedNames>
   <calcPr calcId="140001" concurrentCalc="0"/>
   <extLst>
@@ -34,7 +35,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="6240" uniqueCount="2451">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="6419" uniqueCount="2455">
   <si>
     <t>sonnenburg_culture_num</t>
   </si>
@@ -7387,13 +7388,25 @@
   </si>
   <si>
     <t>Shepherd et al 2018, Varel and Bryant 1974</t>
+  </si>
+  <si>
+    <t>Prepared exactly as previously described.</t>
+  </si>
+  <si>
+    <t>Note: the media listed here are all medias that have been used in this study. In some cases, a microbe was grown in more than one media and metabolomics data are available for those supernatants in Supplementary Table 7.</t>
+  </si>
+  <si>
+    <t>Clostridium spiroforme DSMZ 1552 M1</t>
+  </si>
+  <si>
+    <t>Clostridium spiroforme DSMZ 1552 M2</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <fonts count="5" x14ac:knownFonts="1">
+  <fonts count="6" x14ac:knownFonts="1">
     <font>
       <sz val="12"/>
       <color theme="1"/>
@@ -7430,6 +7443,13 @@
       <family val="2"/>
       <scheme val="minor"/>
     </font>
+    <font>
+      <b/>
+      <sz val="12"/>
+      <color rgb="FF000000"/>
+      <name val="Calibri"/>
+      <scheme val="minor"/>
+    </font>
   </fonts>
   <fills count="2">
     <fill>
@@ -9577,7 +9597,7 @@
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="20">
+  <cellXfs count="22">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="49" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
     <xf numFmtId="49" fontId="1" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1"/>
@@ -9613,6 +9633,12 @@
     <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="left" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="left" wrapText="1"/>
     </xf>
   </cellXfs>
   <cellStyles count="2127">
@@ -12110,6 +12136,919 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+  <dimension ref="A1:A178"/>
+  <sheetViews>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="D30" sqref="D30"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0"/>
+  <cols>
+    <col min="1" max="1" width="48.5" bestFit="1" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:1">
+      <c r="A1" t="s">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="2" spans="1:1">
+      <c r="A2" t="s">
+        <v>1510</v>
+      </c>
+    </row>
+    <row r="3" spans="1:1">
+      <c r="A3" t="s">
+        <v>9</v>
+      </c>
+    </row>
+    <row r="4" spans="1:1">
+      <c r="A4" t="s">
+        <v>360</v>
+      </c>
+    </row>
+    <row r="5" spans="1:1">
+      <c r="A5" t="s">
+        <v>976</v>
+      </c>
+    </row>
+    <row r="6" spans="1:1">
+      <c r="A6" t="s">
+        <v>13</v>
+      </c>
+    </row>
+    <row r="7" spans="1:1">
+      <c r="A7" t="s">
+        <v>15</v>
+      </c>
+    </row>
+    <row r="8" spans="1:1">
+      <c r="A8" t="s">
+        <v>17</v>
+      </c>
+    </row>
+    <row r="9" spans="1:1">
+      <c r="A9" t="s">
+        <v>19</v>
+      </c>
+    </row>
+    <row r="10" spans="1:1">
+      <c r="A10" t="s">
+        <v>977</v>
+      </c>
+    </row>
+    <row r="11" spans="1:1">
+      <c r="A11" t="s">
+        <v>22</v>
+      </c>
+    </row>
+    <row r="12" spans="1:1">
+      <c r="A12" t="s">
+        <v>198</v>
+      </c>
+    </row>
+    <row r="13" spans="1:1">
+      <c r="A13" t="s">
+        <v>196</v>
+      </c>
+    </row>
+    <row r="14" spans="1:1">
+      <c r="A14" t="s">
+        <v>200</v>
+      </c>
+    </row>
+    <row r="15" spans="1:1">
+      <c r="A15" t="s">
+        <v>202</v>
+      </c>
+    </row>
+    <row r="16" spans="1:1">
+      <c r="A16" t="s">
+        <v>204</v>
+      </c>
+    </row>
+    <row r="17" spans="1:1">
+      <c r="A17" t="s">
+        <v>207</v>
+      </c>
+    </row>
+    <row r="18" spans="1:1">
+      <c r="A18" t="s">
+        <v>209</v>
+      </c>
+    </row>
+    <row r="19" spans="1:1">
+      <c r="A19" t="s">
+        <v>211</v>
+      </c>
+    </row>
+    <row r="20" spans="1:1">
+      <c r="A20" t="s">
+        <v>213</v>
+      </c>
+    </row>
+    <row r="21" spans="1:1">
+      <c r="A21" t="s">
+        <v>214</v>
+      </c>
+    </row>
+    <row r="22" spans="1:1">
+      <c r="A22" t="s">
+        <v>218</v>
+      </c>
+    </row>
+    <row r="23" spans="1:1">
+      <c r="A23" t="s">
+        <v>220</v>
+      </c>
+    </row>
+    <row r="24" spans="1:1">
+      <c r="A24" t="s">
+        <v>222</v>
+      </c>
+    </row>
+    <row r="25" spans="1:1">
+      <c r="A25" t="s">
+        <v>224</v>
+      </c>
+    </row>
+    <row r="26" spans="1:1">
+      <c r="A26" t="s">
+        <v>226</v>
+      </c>
+    </row>
+    <row r="27" spans="1:1">
+      <c r="A27" t="s">
+        <v>228</v>
+      </c>
+    </row>
+    <row r="28" spans="1:1">
+      <c r="A28" t="s">
+        <v>230</v>
+      </c>
+    </row>
+    <row r="29" spans="1:1">
+      <c r="A29" t="s">
+        <v>232</v>
+      </c>
+    </row>
+    <row r="30" spans="1:1">
+      <c r="A30" t="s">
+        <v>234</v>
+      </c>
+    </row>
+    <row r="31" spans="1:1">
+      <c r="A31" t="s">
+        <v>237</v>
+      </c>
+    </row>
+    <row r="32" spans="1:1">
+      <c r="A32" t="s">
+        <v>239</v>
+      </c>
+    </row>
+    <row r="33" spans="1:1">
+      <c r="A33" t="s">
+        <v>242</v>
+      </c>
+    </row>
+    <row r="34" spans="1:1">
+      <c r="A34" t="s">
+        <v>244</v>
+      </c>
+    </row>
+    <row r="35" spans="1:1">
+      <c r="A35" t="s">
+        <v>270</v>
+      </c>
+    </row>
+    <row r="36" spans="1:1">
+      <c r="A36" t="s">
+        <v>272</v>
+      </c>
+    </row>
+    <row r="37" spans="1:1">
+      <c r="A37" t="s">
+        <v>274</v>
+      </c>
+    </row>
+    <row r="38" spans="1:1">
+      <c r="A38" t="s">
+        <v>276</v>
+      </c>
+    </row>
+    <row r="39" spans="1:1">
+      <c r="A39" t="s">
+        <v>278</v>
+      </c>
+    </row>
+    <row r="40" spans="1:1">
+      <c r="A40" t="s">
+        <v>280</v>
+      </c>
+    </row>
+    <row r="41" spans="1:1">
+      <c r="A41" t="s">
+        <v>282</v>
+      </c>
+    </row>
+    <row r="42" spans="1:1">
+      <c r="A42" t="s">
+        <v>285</v>
+      </c>
+    </row>
+    <row r="43" spans="1:1">
+      <c r="A43" t="s">
+        <v>248</v>
+      </c>
+    </row>
+    <row r="44" spans="1:1">
+      <c r="A44" t="s">
+        <v>246</v>
+      </c>
+    </row>
+    <row r="45" spans="1:1">
+      <c r="A45" t="s">
+        <v>1701</v>
+      </c>
+    </row>
+    <row r="46" spans="1:1">
+      <c r="A46" t="s">
+        <v>1702</v>
+      </c>
+    </row>
+    <row r="47" spans="1:1">
+      <c r="A47" t="s">
+        <v>1703</v>
+      </c>
+    </row>
+    <row r="48" spans="1:1">
+      <c r="A48" t="s">
+        <v>1704</v>
+      </c>
+    </row>
+    <row r="49" spans="1:1">
+      <c r="A49" t="s">
+        <v>1705</v>
+      </c>
+    </row>
+    <row r="50" spans="1:1">
+      <c r="A50" t="s">
+        <v>1706</v>
+      </c>
+    </row>
+    <row r="51" spans="1:1">
+      <c r="A51" t="s">
+        <v>1707</v>
+      </c>
+    </row>
+    <row r="52" spans="1:1">
+      <c r="A52" t="s">
+        <v>1708</v>
+      </c>
+    </row>
+    <row r="53" spans="1:1">
+      <c r="A53" t="s">
+        <v>1709</v>
+      </c>
+    </row>
+    <row r="54" spans="1:1">
+      <c r="A54" t="s">
+        <v>1710</v>
+      </c>
+    </row>
+    <row r="55" spans="1:1">
+      <c r="A55" t="s">
+        <v>1711</v>
+      </c>
+    </row>
+    <row r="56" spans="1:1">
+      <c r="A56" t="s">
+        <v>1712</v>
+      </c>
+    </row>
+    <row r="57" spans="1:1">
+      <c r="A57" t="s">
+        <v>262</v>
+      </c>
+    </row>
+    <row r="58" spans="1:1">
+      <c r="A58" t="s">
+        <v>266</v>
+      </c>
+    </row>
+    <row r="59" spans="1:1">
+      <c r="A59" t="s">
+        <v>264</v>
+      </c>
+    </row>
+    <row r="60" spans="1:1">
+      <c r="A60" t="s">
+        <v>268</v>
+      </c>
+    </row>
+    <row r="61" spans="1:1">
+      <c r="A61" t="s">
+        <v>307</v>
+      </c>
+    </row>
+    <row r="62" spans="1:1">
+      <c r="A62" t="s">
+        <v>310</v>
+      </c>
+    </row>
+    <row r="63" spans="1:1">
+      <c r="A63" t="s">
+        <v>314</v>
+      </c>
+    </row>
+    <row r="64" spans="1:1">
+      <c r="A64" t="s">
+        <v>312</v>
+      </c>
+    </row>
+    <row r="65" spans="1:1">
+      <c r="A65" t="s">
+        <v>316</v>
+      </c>
+    </row>
+    <row r="66" spans="1:1">
+      <c r="A66" t="s">
+        <v>318</v>
+      </c>
+    </row>
+    <row r="67" spans="1:1">
+      <c r="A67" t="s">
+        <v>320</v>
+      </c>
+    </row>
+    <row r="68" spans="1:1">
+      <c r="A68" t="s">
+        <v>322</v>
+      </c>
+    </row>
+    <row r="69" spans="1:1">
+      <c r="A69" t="s">
+        <v>325</v>
+      </c>
+    </row>
+    <row r="70" spans="1:1">
+      <c r="A70" t="s">
+        <v>978</v>
+      </c>
+    </row>
+    <row r="71" spans="1:1">
+      <c r="A71" t="s">
+        <v>327</v>
+      </c>
+    </row>
+    <row r="72" spans="1:1">
+      <c r="A72" t="s">
+        <v>24</v>
+      </c>
+    </row>
+    <row r="73" spans="1:1">
+      <c r="A73" t="s">
+        <v>979</v>
+      </c>
+    </row>
+    <row r="74" spans="1:1">
+      <c r="A74" t="s">
+        <v>30</v>
+      </c>
+    </row>
+    <row r="75" spans="1:1">
+      <c r="A75" t="s">
+        <v>1512</v>
+      </c>
+    </row>
+    <row r="76" spans="1:1">
+      <c r="A76" t="s">
+        <v>1513</v>
+      </c>
+    </row>
+    <row r="77" spans="1:1">
+      <c r="A77" t="s">
+        <v>346</v>
+      </c>
+    </row>
+    <row r="78" spans="1:1">
+      <c r="A78" t="s">
+        <v>32</v>
+      </c>
+    </row>
+    <row r="79" spans="1:1">
+      <c r="A79" t="s">
+        <v>888</v>
+      </c>
+    </row>
+    <row r="80" spans="1:1">
+      <c r="A80" t="s">
+        <v>981</v>
+      </c>
+    </row>
+    <row r="81" spans="1:1">
+      <c r="A81" t="s">
+        <v>983</v>
+      </c>
+    </row>
+    <row r="82" spans="1:1">
+      <c r="A82" t="s">
+        <v>37</v>
+      </c>
+    </row>
+    <row r="83" spans="1:1">
+      <c r="A83" t="s">
+        <v>39</v>
+      </c>
+    </row>
+    <row r="84" spans="1:1">
+      <c r="A84" t="s">
+        <v>46</v>
+      </c>
+    </row>
+    <row r="85" spans="1:1">
+      <c r="A85" t="s">
+        <v>42</v>
+      </c>
+    </row>
+    <row r="86" spans="1:1">
+      <c r="A86" t="s">
+        <v>44</v>
+      </c>
+    </row>
+    <row r="87" spans="1:1">
+      <c r="A87" t="s">
+        <v>48</v>
+      </c>
+    </row>
+    <row r="88" spans="1:1">
+      <c r="A88" t="s">
+        <v>50</v>
+      </c>
+    </row>
+    <row r="89" spans="1:1">
+      <c r="A89" t="s">
+        <v>52</v>
+      </c>
+    </row>
+    <row r="90" spans="1:1">
+      <c r="A90" t="s">
+        <v>54</v>
+      </c>
+    </row>
+    <row r="91" spans="1:1">
+      <c r="A91" t="s">
+        <v>56</v>
+      </c>
+    </row>
+    <row r="92" spans="1:1">
+      <c r="A92" t="s">
+        <v>58</v>
+      </c>
+    </row>
+    <row r="93" spans="1:1">
+      <c r="A93" t="s">
+        <v>60</v>
+      </c>
+    </row>
+    <row r="94" spans="1:1">
+      <c r="A94" t="s">
+        <v>63</v>
+      </c>
+    </row>
+    <row r="95" spans="1:1">
+      <c r="A95" t="s">
+        <v>66</v>
+      </c>
+    </row>
+    <row r="96" spans="1:1">
+      <c r="A96" t="s">
+        <v>71</v>
+      </c>
+    </row>
+    <row r="97" spans="1:1">
+      <c r="A97" t="s">
+        <v>70</v>
+      </c>
+    </row>
+    <row r="98" spans="1:1">
+      <c r="A98" t="s">
+        <v>73</v>
+      </c>
+    </row>
+    <row r="99" spans="1:1">
+      <c r="A99" t="s">
+        <v>75</v>
+      </c>
+    </row>
+    <row r="100" spans="1:1">
+      <c r="A100" t="s">
+        <v>88</v>
+      </c>
+    </row>
+    <row r="101" spans="1:1">
+      <c r="A101" t="s">
+        <v>2453</v>
+      </c>
+    </row>
+    <row r="102" spans="1:1">
+      <c r="A102" t="s">
+        <v>2454</v>
+      </c>
+    </row>
+    <row r="103" spans="1:1">
+      <c r="A103" t="s">
+        <v>81</v>
+      </c>
+    </row>
+    <row r="104" spans="1:1">
+      <c r="A104" t="s">
+        <v>85</v>
+      </c>
+    </row>
+    <row r="105" spans="1:1">
+      <c r="A105" t="s">
+        <v>83</v>
+      </c>
+    </row>
+    <row r="106" spans="1:1">
+      <c r="A106" t="s">
+        <v>329</v>
+      </c>
+    </row>
+    <row r="107" spans="1:1">
+      <c r="A107" t="s">
+        <v>94</v>
+      </c>
+    </row>
+    <row r="108" spans="1:1">
+      <c r="A108" t="s">
+        <v>97</v>
+      </c>
+    </row>
+    <row r="109" spans="1:1">
+      <c r="A109" t="s">
+        <v>99</v>
+      </c>
+    </row>
+    <row r="110" spans="1:1">
+      <c r="A110" t="s">
+        <v>380</v>
+      </c>
+    </row>
+    <row r="111" spans="1:1">
+      <c r="A111" t="s">
+        <v>377</v>
+      </c>
+    </row>
+    <row r="112" spans="1:1">
+      <c r="A112" t="s">
+        <v>102</v>
+      </c>
+    </row>
+    <row r="113" spans="1:1">
+      <c r="A113" t="s">
+        <v>104</v>
+      </c>
+    </row>
+    <row r="114" spans="1:1">
+      <c r="A114" t="s">
+        <v>349</v>
+      </c>
+    </row>
+    <row r="115" spans="1:1">
+      <c r="A115" t="s">
+        <v>331</v>
+      </c>
+    </row>
+    <row r="116" spans="1:1">
+      <c r="A116" t="s">
+        <v>351</v>
+      </c>
+    </row>
+    <row r="117" spans="1:1">
+      <c r="A117" t="s">
+        <v>106</v>
+      </c>
+    </row>
+    <row r="118" spans="1:1">
+      <c r="A118" t="s">
+        <v>108</v>
+      </c>
+    </row>
+    <row r="119" spans="1:1">
+      <c r="A119" t="s">
+        <v>110</v>
+      </c>
+    </row>
+    <row r="120" spans="1:1">
+      <c r="A120" t="s">
+        <v>112</v>
+      </c>
+    </row>
+    <row r="121" spans="1:1">
+      <c r="A121" t="s">
+        <v>1729</v>
+      </c>
+    </row>
+    <row r="122" spans="1:1">
+      <c r="A122" t="s">
+        <v>117</v>
+      </c>
+    </row>
+    <row r="123" spans="1:1">
+      <c r="A123" t="s">
+        <v>120</v>
+      </c>
+    </row>
+    <row r="124" spans="1:1">
+      <c r="A124" t="s">
+        <v>122</v>
+      </c>
+    </row>
+    <row r="125" spans="1:1">
+      <c r="A125" t="s">
+        <v>125</v>
+      </c>
+    </row>
+    <row r="126" spans="1:1">
+      <c r="A126" t="s">
+        <v>128</v>
+      </c>
+    </row>
+    <row r="127" spans="1:1">
+      <c r="A127" t="s">
+        <v>130</v>
+      </c>
+    </row>
+    <row r="128" spans="1:1">
+      <c r="A128" t="s">
+        <v>132</v>
+      </c>
+    </row>
+    <row r="129" spans="1:1">
+      <c r="A129" t="s">
+        <v>339</v>
+      </c>
+    </row>
+    <row r="130" spans="1:1">
+      <c r="A130" t="s">
+        <v>1722</v>
+      </c>
+    </row>
+    <row r="131" spans="1:1">
+      <c r="A131" t="s">
+        <v>988</v>
+      </c>
+    </row>
+    <row r="132" spans="1:1">
+      <c r="A132" t="s">
+        <v>134</v>
+      </c>
+    </row>
+    <row r="133" spans="1:1">
+      <c r="A133" t="s">
+        <v>987</v>
+      </c>
+    </row>
+    <row r="134" spans="1:1">
+      <c r="A134" t="s">
+        <v>137</v>
+      </c>
+    </row>
+    <row r="135" spans="1:1">
+      <c r="A135" t="s">
+        <v>969</v>
+      </c>
+    </row>
+    <row r="136" spans="1:1">
+      <c r="A136" t="s">
+        <v>963</v>
+      </c>
+    </row>
+    <row r="137" spans="1:1">
+      <c r="A137" t="s">
+        <v>139</v>
+      </c>
+    </row>
+    <row r="138" spans="1:1">
+      <c r="A138" t="s">
+        <v>141</v>
+      </c>
+    </row>
+    <row r="139" spans="1:1">
+      <c r="A139" t="s">
+        <v>145</v>
+      </c>
+    </row>
+    <row r="140" spans="1:1">
+      <c r="A140" t="s">
+        <v>1750</v>
+      </c>
+    </row>
+    <row r="141" spans="1:1">
+      <c r="A141" t="s">
+        <v>147</v>
+      </c>
+    </row>
+    <row r="142" spans="1:1">
+      <c r="A142" t="s">
+        <v>149</v>
+      </c>
+    </row>
+    <row r="143" spans="1:1">
+      <c r="A143" t="s">
+        <v>1730</v>
+      </c>
+    </row>
+    <row r="144" spans="1:1">
+      <c r="A144" t="s">
+        <v>151</v>
+      </c>
+    </row>
+    <row r="145" spans="1:1">
+      <c r="A145" t="s">
+        <v>153</v>
+      </c>
+    </row>
+    <row r="146" spans="1:1">
+      <c r="A146" t="s">
+        <v>155</v>
+      </c>
+    </row>
+    <row r="147" spans="1:1">
+      <c r="A147" t="s">
+        <v>157</v>
+      </c>
+    </row>
+    <row r="148" spans="1:1">
+      <c r="A148" t="s">
+        <v>159</v>
+      </c>
+    </row>
+    <row r="149" spans="1:1">
+      <c r="A149" t="s">
+        <v>162</v>
+      </c>
+    </row>
+    <row r="150" spans="1:1">
+      <c r="A150" t="s">
+        <v>656</v>
+      </c>
+    </row>
+    <row r="151" spans="1:1">
+      <c r="A151" t="s">
+        <v>971</v>
+      </c>
+    </row>
+    <row r="152" spans="1:1">
+      <c r="A152" t="s">
+        <v>989</v>
+      </c>
+    </row>
+    <row r="153" spans="1:1">
+      <c r="A153" t="s">
+        <v>292</v>
+      </c>
+    </row>
+    <row r="154" spans="1:1">
+      <c r="A154" t="s">
+        <v>961</v>
+      </c>
+    </row>
+    <row r="155" spans="1:1">
+      <c r="A155" t="s">
+        <v>296</v>
+      </c>
+    </row>
+    <row r="156" spans="1:1">
+      <c r="A156" t="s">
+        <v>299</v>
+      </c>
+    </row>
+    <row r="157" spans="1:1">
+      <c r="A157" t="s">
+        <v>166</v>
+      </c>
+    </row>
+    <row r="158" spans="1:1">
+      <c r="A158" t="s">
+        <v>300</v>
+      </c>
+    </row>
+    <row r="159" spans="1:1">
+      <c r="A159" t="s">
+        <v>301</v>
+      </c>
+    </row>
+    <row r="160" spans="1:1">
+      <c r="A160" t="s">
+        <v>964</v>
+      </c>
+    </row>
+    <row r="161" spans="1:1">
+      <c r="A161" t="s">
+        <v>304</v>
+      </c>
+    </row>
+    <row r="162" spans="1:1">
+      <c r="A162" t="s">
+        <v>353</v>
+      </c>
+    </row>
+    <row r="163" spans="1:1">
+      <c r="A163" t="s">
+        <v>355</v>
+      </c>
+    </row>
+    <row r="164" spans="1:1">
+      <c r="A164" t="s">
+        <v>357</v>
+      </c>
+    </row>
+    <row r="165" spans="1:1">
+      <c r="A165" t="s">
+        <v>170</v>
+      </c>
+    </row>
+    <row r="166" spans="1:1">
+      <c r="A166" t="s">
+        <v>173</v>
+      </c>
+    </row>
+    <row r="167" spans="1:1">
+      <c r="A167" t="s">
+        <v>175</v>
+      </c>
+    </row>
+    <row r="168" spans="1:1">
+      <c r="A168" t="s">
+        <v>179</v>
+      </c>
+    </row>
+    <row r="169" spans="1:1">
+      <c r="A169" t="s">
+        <v>177</v>
+      </c>
+    </row>
+    <row r="170" spans="1:1">
+      <c r="A170" t="s">
+        <v>990</v>
+      </c>
+    </row>
+    <row r="171" spans="1:1">
+      <c r="A171" t="s">
+        <v>182</v>
+      </c>
+    </row>
+    <row r="172" spans="1:1">
+      <c r="A172" t="s">
+        <v>334</v>
+      </c>
+    </row>
+    <row r="173" spans="1:1">
+      <c r="A173" t="s">
+        <v>992</v>
+      </c>
+    </row>
+    <row r="174" spans="1:1">
+      <c r="A174" t="s">
+        <v>186</v>
+      </c>
+    </row>
+    <row r="175" spans="1:1">
+      <c r="A175" t="s">
+        <v>189</v>
+      </c>
+    </row>
+    <row r="176" spans="1:1">
+      <c r="A176" t="s">
+        <v>967</v>
+      </c>
+    </row>
+    <row r="177" spans="1:1">
+      <c r="A177" t="s">
+        <v>337</v>
+      </c>
+    </row>
+    <row r="178" spans="1:1">
+      <c r="A178" t="s">
+        <v>193</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
+  <extLst>
+    <ext xmlns:mx="http://schemas.microsoft.com/office/mac/excel/2008/main" uri="{64002731-A6B0-56B0-2670-7721B7C09600}">
+      <mx:PLV Mode="0" OnePage="0" WScale="0"/>
+    </ext>
+  </extLst>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:I370"/>
   <sheetViews>
     <sheetView workbookViewId="0">
@@ -21325,7 +22264,7 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:O265"/>
   <sheetViews>
@@ -32560,7 +33499,7 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:B160"/>
   <sheetViews>
@@ -33864,7 +34803,7 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet5.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:C241"/>
   <sheetViews>
@@ -36323,12 +37262,12 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet5.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet6.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:D17"/>
+  <dimension ref="A1:D21"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="A13" sqref="A13"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="B25" sqref="B25"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0"/>
@@ -36392,7 +37331,7 @@
         <v>2419</v>
       </c>
       <c r="D4" s="19" t="s">
-        <v>2417</v>
+        <v>2451</v>
       </c>
     </row>
     <row r="5" spans="1:4">
@@ -36577,7 +37516,24 @@
         <v>2417</v>
       </c>
     </row>
+    <row r="20" spans="1:4">
+      <c r="A20" s="20" t="s">
+        <v>2452</v>
+      </c>
+      <c r="B20" s="21"/>
+      <c r="C20" s="21"/>
+      <c r="D20" s="21"/>
+    </row>
+    <row r="21" spans="1:4">
+      <c r="A21" s="21"/>
+      <c r="B21" s="21"/>
+      <c r="C21" s="21"/>
+      <c r="D21" s="21"/>
+    </row>
   </sheetData>
+  <mergeCells count="1">
+    <mergeCell ref="A20:D21"/>
+  </mergeCells>
   <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
   <pageSetup orientation="portrait" horizontalDpi="4294967292" verticalDpi="4294967292"/>
   <extLst>

</xml_diff>